<commit_message>
saves added to table
</commit_message>
<xml_diff>
--- a/earnings_breakdown.xlsx
+++ b/earnings_breakdown.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>Member</t>
   </si>
@@ -25,10 +25,13 @@
     <t>War_Hits</t>
   </si>
   <si>
+    <t>Total_Score</t>
+  </si>
+  <si>
+    <t>Saves</t>
+  </si>
+  <si>
     <t>Save_Score</t>
-  </si>
-  <si>
-    <t>Total_Score</t>
   </si>
   <si>
     <t>Respect_Share</t>
@@ -698,13 +701,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:L99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -738,10 +741,13 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>2367.69</v>
@@ -750,33 +756,36 @@
         <v>195</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2367.69</v>
       </c>
       <c r="E2">
-        <v>2367.69</v>
+        <v>0</v>
       </c>
       <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <v>6.502792062478921</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>5.68678915135608</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>173344928.0095006</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>75796369.20384952</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>249141297.2133501</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>6.23079109210464</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1901.2</v>
@@ -785,33 +794,36 @@
         <v>185</v>
       </c>
       <c r="D3">
+        <v>1972.36</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
         <v>71.16</v>
       </c>
-      <c r="E3">
-        <v>1972.36</v>
-      </c>
-      <c r="F3">
+      <c r="G3">
         <v>5.417029658591676</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>5.395158938466025</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>144401759.6090783</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>71909375.91134442</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>216311135.5204227</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>5.409739418549791</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>2280.95</v>
@@ -820,33 +832,36 @@
         <v>150</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2280.95</v>
       </c>
       <c r="E4">
-        <v>2280.95</v>
+        <v>0</v>
       </c>
       <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>6.264563162792128</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>4.374453193350831</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>166994460.2305498</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>58304899.38757656</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>225299359.6181263</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>5.634526506311696</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>1752.39</v>
@@ -855,33 +870,36 @@
         <v>142</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1752.39</v>
       </c>
       <c r="E5">
-        <v>1752.39</v>
+        <v>0</v>
       </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>4.812888419669567</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>4.141149023038787</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>128297166.6031316</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>55195304.75357247</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>183492471.3567041</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>4.588975287459307</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>2742.01</v>
@@ -890,33 +908,36 @@
         <v>140</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>2742.01</v>
       </c>
       <c r="E6">
-        <v>2742.01</v>
+        <v>0</v>
       </c>
       <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>7.53085110940952</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>4.082822980460776</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>200749898.0235296</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>54417906.09507145</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>255167804.118601</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>6.381508399759939</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>1410.44</v>
@@ -925,33 +946,36 @@
         <v>115</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1410.44</v>
       </c>
       <c r="E7">
-        <v>1410.44</v>
+        <v>0</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>3.87373264092967</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>3.353747448235637</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>103262091.0092622</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>44700422.86380869</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>147962513.8730709</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>3.700404243364992</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>1055.57</v>
@@ -960,33 +984,36 @@
         <v>97</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1055.57</v>
       </c>
       <c r="E8">
-        <v>1055.57</v>
+        <v>0</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>2.899092456103153</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>2.828813065033537</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>77281107.60234174</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>37703834.9372995</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>114984942.5396412</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>2.875665992413281</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>1212.44</v>
@@ -995,33 +1022,36 @@
         <v>103</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1212.44</v>
       </c>
       <c r="E9">
-        <v>1212.44</v>
+        <v>0</v>
       </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>3.32993137118117</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>3.003791192767571</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>88765980.56157643</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>40036030.91280257</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>128802011.474379</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>3.221217978376636</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>984.72</v>
@@ -1030,33 +1060,36 @@
         <v>93</v>
       </c>
       <c r="D10">
+        <v>1020.3</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
         <v>35.58</v>
       </c>
-      <c r="E10">
-        <v>1020.3</v>
-      </c>
-      <c r="F10">
+      <c r="G10">
         <v>2.802224421840378</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>2.712160979877515</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>74698896.41299893</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>36149037.62029746</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>110847934.0332964</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>2.772203274519423</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>1449.79</v>
@@ -1065,33 +1098,36 @@
         <v>95</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1449.79</v>
       </c>
       <c r="E11">
-        <v>1449.79</v>
+        <v>0</v>
       </c>
       <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
         <v>3.981806277114535</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>2.770487022455526</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>106143009.9290422</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>36926436.27879848</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>143069446.2078407</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>3.578033192228199</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>950.24</v>
@@ -1100,33 +1136,36 @@
         <v>87</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>950.24</v>
       </c>
       <c r="E12">
-        <v>950.24</v>
+        <v>0</v>
       </c>
       <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <v>2.609806659423307</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>2.537182852143482</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>69569616.1202471</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>33816841.6447944</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>103386457.7650415</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>2.585598723663365</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <v>758.87</v>
@@ -1135,33 +1174,36 @@
         <v>86</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>758.87</v>
       </c>
       <c r="E13">
-        <v>758.87</v>
+        <v>0</v>
       </c>
       <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
         <v>2.084214492798203</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>2.508019830854476</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>55558905.73452171</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>33428142.31554389</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>88987048.05006561</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>2.225482938816961</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>977.48</v>
@@ -1170,33 +1212,36 @@
         <v>86</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>977.48</v>
       </c>
       <c r="E14">
-        <v>977.48</v>
+        <v>0</v>
       </c>
       <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
         <v>2.684620531079616</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>2.508019830854476</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>71563929.49698931</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>33428142.31554389</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>104992071.8125332</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>2.625753631004569</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>741.27</v>
@@ -1205,33 +1250,36 @@
         <v>82</v>
       </c>
       <c r="D15">
+        <v>764.99</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
         <v>23.72</v>
       </c>
-      <c r="E15">
-        <v>764.99</v>
-      </c>
-      <c r="F15">
+      <c r="G15">
         <v>2.101022895681339</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>2.391367745698454</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>56006967.33017745</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>31873344.99854185</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>87880312.3287193</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>2.197804512353711</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>944.9299999999999</v>
@@ -1240,33 +1288,36 @@
         <v>77</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>944.9299999999999</v>
       </c>
       <c r="E16">
-        <v>944.9299999999999</v>
+        <v>0</v>
       </c>
       <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
         <v>2.595222898098233</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>2.245552639253427</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>69180856.7946046</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>29929848.3522893</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>99110705.1468939</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>2.478666145149965</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>671.1799999999999</v>
@@ -1275,33 +1326,36 @@
         <v>74</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>671.1799999999999</v>
       </c>
       <c r="E17">
-        <v>671.1799999999999</v>
+        <v>0</v>
       </c>
       <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
         <v>1.843376445605042</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>2.15806357538641</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>49138885.9104936</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>28763750.36453777</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>77902636.27503136</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>1.948272155532164</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>861.28</v>
@@ -1310,33 +1364,36 @@
         <v>70</v>
       </c>
       <c r="D18">
+        <v>873.14</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
         <v>11.86</v>
       </c>
-      <c r="E18">
-        <v>873.14</v>
-      </c>
-      <c r="F18">
+      <c r="G18">
         <v>2.398053740748512</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>2.041411490230388</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>63924918.56713308</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>27208953.04753572</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>91133871.61466882</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>2.279172990575804</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <v>494.76</v>
@@ -1345,33 +1402,36 @@
         <v>65</v>
       </c>
       <c r="D19">
+        <v>554.0599999999999</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
         <v>59.3</v>
       </c>
-      <c r="E19">
-        <v>554.0599999999999</v>
-      </c>
-      <c r="F19">
+      <c r="G19">
         <v>1.521709755135626</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>1.89559638378536</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>40564216.94265038</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>25265456.40128317</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>65829673.34393355</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>1.646338631352204</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <v>543.72</v>
@@ -1380,33 +1440,36 @@
         <v>61</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>543.72</v>
       </c>
       <c r="E20">
-        <v>543.72</v>
+        <v>0</v>
       </c>
       <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
         <v>1.493311244382094</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>1.778944298629338</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>39807197.84149347</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>23710659.08428113</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>63517856.9257746</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>1.588522262464508</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21">
         <v>437.05</v>
@@ -1415,33 +1478,36 @@
         <v>63</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>437.05</v>
       </c>
       <c r="E21">
-        <v>437.05</v>
+        <v>0</v>
       </c>
       <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
         <v>1.200345176482737</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>1.837270341207349</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>31997601.36950033</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>24488057.74278215</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>56485659.11228248</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>1.412653564724275</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22">
         <v>466.79</v>
@@ -1450,33 +1516,36 @@
         <v>59</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>466.79</v>
       </c>
       <c r="E22">
-        <v>466.79</v>
+        <v>0</v>
       </c>
       <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
         <v>1.282025225787386</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>1.720618256051327</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>34174946.44381434</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>22933260.42578011</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>57108206.86959445</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>1.428222902542033</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23">
         <v>502.66</v>
@@ -1485,33 +1554,36 @@
         <v>62</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>502.66</v>
       </c>
       <c r="E23">
-        <v>502.66</v>
+        <v>0</v>
       </c>
       <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
         <v>1.380541142685763</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>1.808107319918344</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>36801085.24057438</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>24099358.41353164</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>60900443.65410602</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>1.52306320176329</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>624.22</v>
@@ -1520,33 +1592,36 @@
         <v>59</v>
       </c>
       <c r="D24">
+        <v>636.08</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
         <v>11.86</v>
       </c>
-      <c r="E24">
-        <v>636.08</v>
-      </c>
-      <c r="F24">
+      <c r="G24">
         <v>1.746975311422353</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>1.720618256051327</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>46569120.87658568</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>22933260.42578011</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>69502381.30236579</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>1.738189626298678</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25">
         <v>474.91</v>
@@ -1555,33 +1630,36 @@
         <v>54</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>474.91</v>
       </c>
       <c r="E25">
-        <v>474.91</v>
+        <v>0</v>
       </c>
       <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
         <v>1.304326570789193</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>1.574803149606299</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>34769433.39752752</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>20989763.77952756</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>55759197.17705508</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>1.394485430394895</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>410.97</v>
@@ -1590,33 +1668,36 @@
         <v>53</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>410.97</v>
       </c>
       <c r="E26">
-        <v>410.97</v>
+        <v>0</v>
       </c>
       <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
         <v>1.128717211255258</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>1.545640128317294</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>30088214.70043141</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>20601064.45027705</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>50689279.15070847</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>1.267691516942604</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <v>505.47</v>
@@ -1625,33 +1706,36 @@
         <v>51</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>505.47</v>
       </c>
       <c r="E27">
-        <v>505.47</v>
+        <v>0</v>
       </c>
       <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
         <v>1.388258726362497</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>1.487314085739283</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>37006812.86864508</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>19823665.79177603</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>56830478.6604211</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>1.421277179488092</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28">
         <v>659.3200000000001</v>
@@ -1660,33 +1744,36 @@
         <v>52</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>659.3200000000001</v>
       </c>
       <c r="E28">
-        <v>659.3200000000001</v>
+        <v>0</v>
       </c>
       <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
         <v>1.810803298841319</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>1.516477107028288</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>48270583.53721303</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>20212365.12102654</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>68482948.65823957</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>1.712694568236975</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B29">
         <v>482.57</v>
@@ -1695,33 +1782,36 @@
         <v>51</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>482.57</v>
       </c>
       <c r="E29">
-        <v>482.57</v>
+        <v>0</v>
       </c>
       <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
         <v>1.325364539103706</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>1.487314085739283</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>35330242.51888748</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>19823665.79177603</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>55153908.31066351</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>1.379347721315565</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B30">
         <v>343.82</v>
@@ -1730,33 +1820,36 @@
         <v>51</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>343.82</v>
       </c>
       <c r="E30">
-        <v>343.82</v>
+        <v>0</v>
       </c>
       <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
         <v>0.9442916796208551</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>1.487314085739283</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>25171983.30365313</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>19823665.79177603</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>44995649.09542916</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>1.125299148326997</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B31">
         <v>512.83</v>
@@ -1765,33 +1858,36 @@
         <v>50</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>512.83</v>
       </c>
       <c r="E31">
-        <v>512.83</v>
+        <v>0</v>
       </c>
       <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
         <v>1.408472753359209</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>1.458151064450277</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>37545658.18629643</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>19434966.46252552</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>56980624.64882195</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>1.425032190389565</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B32">
         <v>327.71</v>
@@ -1800,33 +1896,36 @@
         <v>36</v>
       </c>
       <c r="D32">
+        <v>339.57</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
         <v>11.86</v>
       </c>
-      <c r="E32">
-        <v>339.57</v>
-      </c>
-      <c r="F32">
+      <c r="G32">
         <v>0.9326191776186777</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>1.049868766404199</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>24860829.41778109</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>13993175.85301837</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>38854005.27079947</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>0.9717023738805184</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B33">
         <v>498.69</v>
@@ -1835,33 +1934,36 @@
         <v>44</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>498.69</v>
       </c>
       <c r="E33">
-        <v>498.69</v>
+        <v>0</v>
       </c>
       <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
         <v>1.3696376525802</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>1.283172936716244</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>36510430.90483038</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>17102770.48702246</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>53613201.39185284</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>1.340816080625548</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B34">
         <v>186.59</v>
@@ -1870,33 +1972,36 @@
         <v>40</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>186.59</v>
       </c>
       <c r="E34">
-        <v>186.59</v>
+        <v>0</v>
       </c>
       <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
         <v>0.512464034961478</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>1.166520851560222</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>13660753.77996812</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>15547973.17002041</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>29208726.94998853</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>0.7304829738277259</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B35">
         <v>286.64</v>
@@ -1905,33 +2010,36 @@
         <v>28</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>286.64</v>
       </c>
       <c r="E35">
-        <v>286.64</v>
+        <v>0</v>
       </c>
       <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
         <v>0.7872484644480306</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>0.8165645960921551</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>20985682.31679115</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>10883581.21901429</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>31869263.53580544</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>0.7970205083294055</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B36">
         <v>253.73</v>
@@ -1940,33 +2048,36 @@
         <v>34</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>253.73</v>
       </c>
       <c r="E36">
-        <v>253.73</v>
+        <v>0</v>
       </c>
       <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
         <v>0.6968621018852875</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>0.9915427238261884</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>18576253.04995611</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>13215777.19451735</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>31792030.24447346</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>0.7950889758655879</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B37">
         <v>232.53</v>
@@ -1975,33 +2086,36 @@
         <v>36</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>232.53</v>
       </c>
       <c r="E37">
-        <v>232.53</v>
+        <v>0</v>
       </c>
       <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
         <v>0.6386369154273674</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>1.049868766404199</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>17024144.25454733</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>13993175.85301837</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>31017320.1075657</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>0.7757141990863115</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B38">
         <v>334.46</v>
@@ -2010,33 +2124,36 @@
         <v>35</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>334.46</v>
       </c>
       <c r="E38">
-        <v>334.46</v>
+        <v>0</v>
       </c>
       <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
         <v>0.9185847105054714</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>1.020705745115194</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>24486712.62794435</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>13604476.52376786</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>38091189.15171221</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>0.9526250553753788</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B39">
         <v>389.89</v>
@@ -2045,33 +2162,36 @@
         <v>34</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>389.89</v>
       </c>
       <c r="E39">
-        <v>389.89</v>
+        <v>0</v>
       </c>
       <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
         <v>1.070821601324458</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>0.9915427238261884</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>28544891.42650608</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>13215777.19451735</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>41760668.62102343</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>1.044395308825035</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B40">
         <v>140.88</v>
@@ -2080,33 +2200,36 @@
         <v>22</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>140.88</v>
       </c>
       <c r="E40">
-        <v>140.88</v>
+        <v>0</v>
       </c>
       <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
         <v>0.3869228428392358</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>0.6415864683581218</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>10314202.22156551</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>8551385.243511228</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>18865587.46507674</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>0.4718107180121978</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <v>25.14</v>
@@ -2115,33 +2238,36 @@
         <v>2</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>25.14</v>
       </c>
       <c r="E41">
-        <v>25.14</v>
+        <v>0</v>
       </c>
       <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
         <v>0.06904628243170351</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>0.05832604257801108</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>1840566.75078192</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>777398.6585010207</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>2617965.409282941</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>0.06547286914713936</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B42">
         <v>260.88</v>
@@ -2150,33 +2276,36 @@
         <v>26</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>260.88</v>
       </c>
       <c r="E42">
-        <v>260.88</v>
+        <v>0</v>
       </c>
       <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
         <v>0.716499369959539</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>0.758238553514144</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>19099723.70501143</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>10106182.56051327</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>29205906.2655247</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>0.7304124311444072</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -2208,10 +2337,13 @@
       <c r="K43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="L43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B44">
         <v>214.4</v>
@@ -2220,33 +2352,36 @@
         <v>25</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>214.4</v>
       </c>
       <c r="E44">
-        <v>214.4</v>
+        <v>0</v>
       </c>
       <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
         <v>0.5888433951216082</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>0.7290755322251385</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>15696798.38375671</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>9717483.23126276</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>25414281.61501947</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>0.635587440822785</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B45">
         <v>98.95999999999999</v>
@@ -2255,33 +2390,36 @@
         <v>19</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>98.95999999999999</v>
       </c>
       <c r="E45">
-        <v>98.95999999999999</v>
+        <v>0</v>
       </c>
       <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
         <v>0.2717907760318766</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>0.5540974044911053</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>7245126.716681735</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <v>7385287.255759697</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>14630413.97244143</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>0.3658929855182861</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B46">
         <v>284.4</v>
@@ -2290,33 +2428,36 @@
         <v>24</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>284.4</v>
       </c>
       <c r="E46">
-        <v>284.4</v>
+        <v>0</v>
       </c>
       <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
         <v>0.7810963692751184</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>0.699912510936133</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>20821685.91576683</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>9328783.902012249</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>30150469.81777908</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <v>0.7540350831621232</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B47">
         <v>167.51</v>
@@ -2325,33 +2466,36 @@
         <v>24</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>167.51</v>
       </c>
       <c r="E47">
-        <v>167.51</v>
+        <v>0</v>
       </c>
       <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
         <v>0.4600613671493498</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>0.699912510936133</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>12263855.86410022</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>9328783.902012249</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>21592639.76611247</v>
       </c>
-      <c r="K47">
+      <c r="L47">
         <v>0.5400117484116108</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B48">
         <v>232.64</v>
@@ -2360,33 +2504,36 @@
         <v>23</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>232.64</v>
       </c>
       <c r="E48">
-        <v>232.64</v>
+        <v>0</v>
       </c>
       <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
         <v>0.6389390272438943</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>0.6707494896471274</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>17032197.64924049</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>8940084.572761739</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>25972282.22200223</v>
       </c>
-      <c r="K48">
+      <c r="L48">
         <v>0.6495425147116387</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B49">
         <v>135.41</v>
@@ -2395,33 +2542,36 @@
         <v>17</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>135.41</v>
       </c>
       <c r="E49">
-        <v>135.41</v>
+        <v>0</v>
       </c>
       <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
         <v>0.3718996461446687</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>0.4957713619130942</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>9913728.867278432</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>6607888.597258677</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>16521617.46453711</v>
       </c>
-      <c r="K49">
+      <c r="L49">
         <v>0.4131902180674772</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B50">
         <v>166.9</v>
@@ -2430,33 +2580,36 @@
         <v>21</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>166.9</v>
       </c>
       <c r="E50">
-        <v>166.9</v>
+        <v>0</v>
       </c>
       <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
         <v>0.4583860198031549</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>0.6124234470691163</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <v>12219196.1298927</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>8162685.914260718</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>20381882.04415342</v>
       </c>
-      <c r="K50">
+      <c r="L50">
         <v>0.5097318288918087</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B51">
         <v>101.81</v>
@@ -2465,33 +2618,36 @@
         <v>21</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>101.81</v>
       </c>
       <c r="E51">
-        <v>101.81</v>
+        <v>0</v>
       </c>
       <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
         <v>0.2796182185509838</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>0.6124234470691163</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>7453782.851913576</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <v>8162685.914260718</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>15616468.76617429</v>
       </c>
-      <c r="K51">
+      <c r="L51">
         <v>0.3905532947236947</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B52">
         <v>170.22</v>
@@ -2500,33 +2656,36 @@
         <v>21</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>170.22</v>
       </c>
       <c r="E52">
-        <v>170.22</v>
+        <v>0</v>
       </c>
       <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
         <v>0.46750430372015</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>0.6124234470691163</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>12462262.22426804</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>8162685.914260718</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>20624948.13852875</v>
       </c>
-      <c r="K52">
+      <c r="L52">
         <v>0.5158106848364721</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B53">
         <v>114.72</v>
@@ -2535,33 +2694,36 @@
         <v>20</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>114.72</v>
       </c>
       <c r="E53">
-        <v>114.72</v>
+        <v>0</v>
       </c>
       <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
         <v>0.3150751599270098</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>0.5832604257801108</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>8398958.5381743</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>7773986.585010207</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>16172945.12318451</v>
       </c>
-      <c r="K53">
+      <c r="L53">
         <v>0.4044702485447101</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B54">
         <v>181.86</v>
@@ -2570,33 +2732,36 @@
         <v>20</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>181.86</v>
       </c>
       <c r="E54">
-        <v>181.86</v>
+        <v>0</v>
       </c>
       <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
         <v>0.4994732268508194</v>
       </c>
-      <c r="G54">
+      <c r="H54">
         <v>0.5832604257801108</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <v>13314457.80816229</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>7773986.585010207</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>21088444.3931725</v>
       </c>
-      <c r="K54">
+      <c r="L54">
         <v>0.5274022931605832</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B55">
         <v>259.41</v>
@@ -2605,33 +2770,36 @@
         <v>19</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>259.41</v>
       </c>
       <c r="E55">
-        <v>259.41</v>
+        <v>0</v>
       </c>
       <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
         <v>0.7124620575023153</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>0.5540974044911053</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>18992101.06683922</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <v>7385287.255759697</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>26377388.32259892</v>
       </c>
-      <c r="K55">
+      <c r="L55">
         <v>0.659673839831912</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B56">
         <v>144.92</v>
@@ -2640,33 +2808,36 @@
         <v>18</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>144.92</v>
       </c>
       <c r="E56">
-        <v>144.92</v>
+        <v>0</v>
       </c>
       <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
         <v>0.3980185859189527</v>
       </c>
-      <c r="G56">
+      <c r="H56">
         <v>0.5249343832020997</v>
       </c>
-      <c r="H56">
+      <c r="I56">
         <v>10609981.44484152</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <v>6996587.926509187</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>17606569.37135071</v>
       </c>
-      <c r="K56">
+      <c r="L56">
         <v>0.4403238516800017</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B57">
         <v>155.96</v>
@@ -2675,33 +2846,36 @@
         <v>15</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>155.96</v>
       </c>
       <c r="E57">
-        <v>155.96</v>
+        <v>0</v>
       </c>
       <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
         <v>0.4283396264140206</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>0.4374453193350831</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <v>11418249.42131855</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <v>5830489.938757655</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>17248739.3600762</v>
       </c>
-      <c r="K57">
+      <c r="L57">
         <v>0.4313748573877081</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B58">
         <v>122.35</v>
@@ -2710,33 +2884,36 @@
         <v>17</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>122.35</v>
       </c>
       <c r="E58">
-        <v>122.35</v>
+        <v>0</v>
       </c>
       <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
         <v>0.3360307341097424</v>
       </c>
-      <c r="G58">
+      <c r="H58">
         <v>0.4957713619130942</v>
       </c>
-      <c r="H58">
+      <c r="I58">
         <v>8957571.279163402</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <v>6607888.597258677</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <v>15565459.87642208</v>
       </c>
-      <c r="K58">
+      <c r="L58">
         <v>0.389277610044193</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B59">
         <v>86.54000000000001</v>
@@ -2745,33 +2922,36 @@
         <v>10</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>86.54000000000001</v>
       </c>
       <c r="E59">
-        <v>86.54000000000001</v>
+        <v>0</v>
       </c>
       <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
         <v>0.2376796054749253</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>0.2916302128900554</v>
       </c>
-      <c r="H59">
+      <c r="I59">
         <v>6335825.243145083</v>
       </c>
-      <c r="I59">
+      <c r="J59">
         <v>3886993.292505104</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>10222818.53565019</v>
       </c>
-      <c r="K59">
+      <c r="L59">
         <v>0.2556631412799686</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B60">
         <v>65.93000000000001</v>
@@ -2780,33 +2960,36 @@
         <v>14</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>65.93000000000001</v>
       </c>
       <c r="E60">
-        <v>65.93000000000001</v>
+        <v>0</v>
       </c>
       <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
         <v>0.1810748369420132</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>0.4082822980460776</v>
       </c>
-      <c r="H60">
+      <c r="I60">
         <v>4826911.928363246</v>
       </c>
-      <c r="I60">
+      <c r="J60">
         <v>5441790.609507145</v>
       </c>
-      <c r="J60">
+      <c r="K60">
         <v>10268702.53787039</v>
       </c>
-      <c r="K60">
+      <c r="L60">
         <v>0.2568106573100347</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B61">
         <v>81.84999999999999</v>
@@ -2815,33 +2998,36 @@
         <v>14</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>81.84999999999999</v>
       </c>
       <c r="E61">
-        <v>81.84999999999999</v>
+        <v>0</v>
       </c>
       <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
         <v>0.2247986562066401</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>0.4082822980460776</v>
       </c>
-      <c r="H61">
+      <c r="I61">
         <v>5992457.778500404</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <v>5441790.609507145</v>
       </c>
-      <c r="J61">
+      <c r="K61">
         <v>11434248.38800755</v>
       </c>
-      <c r="K61">
+      <c r="L61">
         <v>0.2859598701531192</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B62">
         <v>14.79</v>
@@ -2850,33 +3036,36 @@
         <v>2</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>14.79</v>
       </c>
       <c r="E62">
-        <v>14.79</v>
+        <v>0</v>
       </c>
       <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
         <v>0.04062030696757735</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>0.05832604257801108</v>
       </c>
-      <c r="H62">
+      <c r="I62">
         <v>1082815.52283471</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <v>777398.6585010207</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>1860214.18133573</v>
       </c>
-      <c r="K62">
+      <c r="L62">
         <v>0.04652221883772194</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B63">
         <v>91.64</v>
@@ -2885,33 +3074,36 @@
         <v>12</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>91.64</v>
       </c>
       <c r="E63">
-        <v>91.64</v>
+        <v>0</v>
       </c>
       <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
         <v>0.2516866078775382</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>0.3499562554680665</v>
       </c>
-      <c r="H63">
+      <c r="I63">
         <v>6709209.906191534</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>4664391.951006125</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <v>11373601.85719766</v>
       </c>
-      <c r="K63">
+      <c r="L63">
         <v>0.2844431570743809</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B64">
         <v>78.70999999999999</v>
@@ -2920,33 +3112,36 @@
         <v>12</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>78.70999999999999</v>
       </c>
       <c r="E64">
-        <v>78.70999999999999</v>
+        <v>0</v>
       </c>
       <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
         <v>0.2161747370803255</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>0.3499562554680665</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <v>5762569.966350236</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <v>4664391.951006125</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>10426961.91735636</v>
       </c>
-      <c r="K64">
+      <c r="L64">
         <v>0.2607685765429058</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B65">
         <v>118.86</v>
@@ -2955,33 +3150,36 @@
         <v>12</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>118.86</v>
       </c>
       <c r="E65">
-        <v>118.86</v>
+        <v>0</v>
       </c>
       <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
         <v>0.3264455501126602</v>
       </c>
-      <c r="G65">
+      <c r="H65">
         <v>0.3499562554680665</v>
       </c>
-      <c r="H65">
+      <c r="I65">
         <v>8702059.029353183</v>
       </c>
-      <c r="I65">
+      <c r="J65">
         <v>4664391.951006125</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <v>13366450.98035931</v>
       </c>
-      <c r="K65">
+      <c r="L65">
         <v>0.3342824518977957</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B66">
         <v>90.81</v>
@@ -2990,33 +3188,36 @@
         <v>10</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>90.81</v>
       </c>
       <c r="E66">
-        <v>90.81</v>
+        <v>0</v>
       </c>
       <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
         <v>0.2494070368982894</v>
       </c>
-      <c r="G66">
+      <c r="H66">
         <v>0.2916302128900554</v>
       </c>
-      <c r="H66">
+      <c r="I66">
         <v>6648443.3825977</v>
       </c>
-      <c r="I66">
+      <c r="J66">
         <v>3886993.292505104</v>
       </c>
-      <c r="J66">
+      <c r="K66">
         <v>10535436.6751028</v>
       </c>
-      <c r="K66">
+      <c r="L66">
         <v>0.2634814288955447</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -3048,10 +3249,13 @@
       <c r="K67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:11">
+      <c r="L67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B68">
         <v>9.640000000000001</v>
@@ -3060,33 +3264,36 @@
         <v>1</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="E68">
-        <v>9.640000000000001</v>
+        <v>0</v>
       </c>
       <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
         <v>0.02647598101199768</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>0.02916302128900554</v>
       </c>
-      <c r="H68">
+      <c r="I68">
         <v>705770.2258368223</v>
       </c>
-      <c r="I68">
+      <c r="J68">
         <v>388699.3292505104</v>
       </c>
-      <c r="J68">
+      <c r="K68">
         <v>1094469.555087333</v>
       </c>
-      <c r="K68">
+      <c r="L68">
         <v>0.02737166110433363</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B69">
         <v>51.9</v>
@@ -3095,33 +3302,36 @@
         <v>7</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>51.9</v>
       </c>
       <c r="E69">
-        <v>51.9</v>
+        <v>0</v>
       </c>
       <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
         <v>0.1425418479795311</v>
       </c>
-      <c r="G69">
+      <c r="H69">
         <v>0.2041411490230388</v>
       </c>
-      <c r="H69">
+      <c r="I69">
         <v>3799738.04159036</v>
       </c>
-      <c r="I69">
+      <c r="J69">
         <v>2720895.304753573</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <v>6520633.346343933</v>
       </c>
-      <c r="K69">
+      <c r="L69">
         <v>0.163074948327367</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B70">
         <v>39.43</v>
@@ -3130,33 +3340,36 @@
         <v>7</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>39.43</v>
       </c>
       <c r="E70">
-        <v>39.43</v>
+        <v>0</v>
       </c>
       <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
         <v>0.1082933538696129</v>
       </c>
-      <c r="G70">
+      <c r="H70">
         <v>0.2041411490230388</v>
       </c>
-      <c r="H70">
+      <c r="I70">
         <v>2886775.934102272</v>
       </c>
-      <c r="I70">
+      <c r="J70">
         <v>2720895.304753573</v>
       </c>
-      <c r="J70">
+      <c r="K70">
         <v>5607671.238855844</v>
       </c>
-      <c r="K70">
+      <c r="L70">
         <v>0.1402426189207549</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B71">
         <v>33.28</v>
@@ -3165,33 +3378,36 @@
         <v>7</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>33.28</v>
       </c>
       <c r="E71">
-        <v>33.28</v>
+        <v>0</v>
       </c>
       <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
         <v>0.09140255685469739</v>
       </c>
-      <c r="G71">
+      <c r="H71">
         <v>0.2041411490230388</v>
       </c>
-      <c r="H71">
+      <c r="I71">
         <v>2436517.958075669</v>
       </c>
-      <c r="I71">
+      <c r="J71">
         <v>2720895.304753573</v>
       </c>
-      <c r="J71">
+      <c r="K71">
         <v>5157413.262829241</v>
       </c>
-      <c r="K71">
+      <c r="L71">
         <v>0.1289820875774779</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -3223,10 +3439,13 @@
       <c r="K72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:11">
+      <c r="L72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B73">
         <v>42.1</v>
@@ -3235,33 +3454,36 @@
         <v>6</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>42.1</v>
       </c>
       <c r="E73">
-        <v>42.1</v>
+        <v>0</v>
       </c>
       <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
         <v>0.1156264315980397</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>0.1749781277340333</v>
       </c>
-      <c r="H73">
+      <c r="I73">
         <v>3082253.787108943</v>
       </c>
-      <c r="I73">
+      <c r="J73">
         <v>2332195.975503062</v>
       </c>
-      <c r="J73">
+      <c r="K73">
         <v>5414449.762612006</v>
       </c>
-      <c r="K73">
+      <c r="L73">
         <v>0.1354103303100375</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:12">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B74">
         <v>43.78</v>
@@ -3270,33 +3492,36 @@
         <v>6</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>43.78</v>
       </c>
       <c r="E74">
-        <v>43.78</v>
+        <v>0</v>
       </c>
       <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
         <v>0.1202405029777239</v>
       </c>
-      <c r="G74">
+      <c r="H74">
         <v>0.1749781277340333</v>
       </c>
-      <c r="H74">
+      <c r="I74">
         <v>3205251.087877186</v>
       </c>
-      <c r="I74">
+      <c r="J74">
         <v>2332195.975503062</v>
       </c>
-      <c r="J74">
+      <c r="K74">
         <v>5537447.063380249</v>
       </c>
-      <c r="K74">
+      <c r="L74">
         <v>0.1384863778964937</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:12">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B75">
         <v>55.26</v>
@@ -3305,33 +3530,36 @@
         <v>6</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>55.26</v>
       </c>
       <c r="E75">
-        <v>55.26</v>
+        <v>0</v>
       </c>
       <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
         <v>0.1517699907388996</v>
       </c>
-      <c r="G75">
+      <c r="H75">
         <v>0.1749781277340333</v>
       </c>
-      <c r="H75">
+      <c r="I75">
         <v>4045732.643126846</v>
       </c>
-      <c r="I75">
+      <c r="J75">
         <v>2332195.975503062</v>
       </c>
-      <c r="J75">
+      <c r="K75">
         <v>6377928.618629908</v>
       </c>
-      <c r="K75">
+      <c r="L75">
         <v>0.1595060364039441</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:12">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B76">
         <v>59.08</v>
@@ -3340,33 +3568,36 @@
         <v>6</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>59.08</v>
       </c>
       <c r="E76">
-        <v>59.08</v>
+        <v>0</v>
       </c>
       <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
         <v>0.1622615101855626</v>
       </c>
-      <c r="G76">
+      <c r="H76">
         <v>0.1749781277340333</v>
       </c>
-      <c r="H76">
+      <c r="I76">
         <v>4325405.077016541</v>
       </c>
-      <c r="I76">
+      <c r="J76">
         <v>2332195.975503062</v>
       </c>
-      <c r="J76">
+      <c r="K76">
         <v>6657601.052519603</v>
       </c>
-      <c r="K76">
+      <c r="L76">
         <v>0.1665003827017195</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:12">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B77">
         <v>6.3</v>
@@ -3375,33 +3606,36 @@
         <v>1</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>6.3</v>
       </c>
       <c r="E77">
-        <v>6.3</v>
+        <v>0</v>
       </c>
       <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
         <v>0.01730276767381591</v>
       </c>
-      <c r="G77">
+      <c r="H77">
         <v>0.02916302128900554</v>
       </c>
-      <c r="H77">
+      <c r="I77">
         <v>461239.8778809108</v>
       </c>
-      <c r="I77">
+      <c r="J77">
         <v>388699.3292505104</v>
       </c>
-      <c r="J77">
+      <c r="K77">
         <v>849939.2071314212</v>
       </c>
-      <c r="K77">
+      <c r="L77">
         <v>0.02125618554554579</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:12">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B78">
         <v>41.22</v>
@@ -3410,33 +3644,36 @@
         <v>5</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>41.22</v>
       </c>
       <c r="E78">
-        <v>41.22</v>
+        <v>0</v>
       </c>
       <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
         <v>0.1132095370658241</v>
       </c>
-      <c r="G78">
+      <c r="H78">
         <v>0.1458151064450277</v>
       </c>
-      <c r="H78">
+      <c r="I78">
         <v>3017826.629563673</v>
       </c>
-      <c r="I78">
+      <c r="J78">
         <v>1943496.646252552</v>
       </c>
-      <c r="J78">
+      <c r="K78">
         <v>4961323.275816225</v>
       </c>
-      <c r="K78">
+      <c r="L78">
         <v>0.1240780601922253</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:12">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B79">
         <v>27.92</v>
@@ -3445,33 +3682,36 @@
         <v>4</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>27.92</v>
       </c>
       <c r="E79">
-        <v>27.92</v>
+        <v>0</v>
       </c>
       <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
         <v>0.0766814719766572</v>
       </c>
-      <c r="G79">
+      <c r="H79">
         <v>0.1166520851560222</v>
       </c>
-      <c r="H79">
+      <c r="I79">
         <v>2044097.998481751</v>
       </c>
-      <c r="I79">
+      <c r="J79">
         <v>1554797.317002041</v>
       </c>
-      <c r="J79">
+      <c r="K79">
         <v>3598895.315483792</v>
       </c>
-      <c r="K79">
+      <c r="L79">
         <v>0.09000500970311219</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:12">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B80">
         <v>16.63</v>
@@ -3480,33 +3720,36 @@
         <v>4</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>16.63</v>
       </c>
       <c r="E80">
-        <v>16.63</v>
+        <v>0</v>
       </c>
       <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
         <v>0.04567381371675534</v>
       </c>
-      <c r="G80">
+      <c r="H80">
         <v>0.1166520851560222</v>
       </c>
-      <c r="H80">
+      <c r="I80">
         <v>1217526.852247547</v>
       </c>
-      <c r="I80">
+      <c r="J80">
         <v>1554797.317002041</v>
       </c>
-      <c r="J80">
+      <c r="K80">
         <v>2772324.169249589</v>
       </c>
-      <c r="K80">
+      <c r="L80">
         <v>0.06933323752984429</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:12">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B81">
         <v>11.06</v>
@@ -3515,33 +3758,36 @@
         <v>2</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>11.06</v>
       </c>
       <c r="E81">
-        <v>11.06</v>
+        <v>0</v>
       </c>
       <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
         <v>0.03037596991625461</v>
       </c>
-      <c r="G81">
+      <c r="H81">
         <v>0.05832604257801108</v>
       </c>
-      <c r="H81">
+      <c r="I81">
         <v>809732.2300575989</v>
       </c>
-      <c r="I81">
+      <c r="J81">
         <v>777398.6585010207</v>
       </c>
-      <c r="J81">
+      <c r="K81">
         <v>1587130.88855862</v>
       </c>
-      <c r="K81">
+      <c r="L81">
         <v>0.03969266080350677</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:12">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B82">
         <v>11.4</v>
@@ -3550,33 +3796,36 @@
         <v>3</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>11.4</v>
       </c>
       <c r="E82">
-        <v>11.4</v>
+        <v>0</v>
       </c>
       <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
         <v>0.0313097700764288</v>
       </c>
-      <c r="G82">
+      <c r="H82">
         <v>0.08748906386701663</v>
       </c>
-      <c r="H82">
+      <c r="I82">
         <v>834624.5409273624</v>
       </c>
-      <c r="I82">
+      <c r="J82">
         <v>1166097.987751531</v>
       </c>
-      <c r="J82">
+      <c r="K82">
         <v>2000722.528678894</v>
       </c>
-      <c r="K82">
+      <c r="L82">
         <v>0.05003620133995808</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:12">
       <c r="A83" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B83">
         <v>36.22</v>
@@ -3585,33 +3834,36 @@
         <v>3</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>36.22</v>
       </c>
       <c r="E83">
-        <v>36.22</v>
+        <v>0</v>
       </c>
       <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
         <v>0.09947718176914482</v>
       </c>
-      <c r="G83">
+      <c r="H83">
         <v>0.08748906386701663</v>
       </c>
-      <c r="H83">
+      <c r="I83">
         <v>2651763.234420093</v>
       </c>
-      <c r="I83">
+      <c r="J83">
         <v>1166097.987751531</v>
       </c>
-      <c r="J83">
+      <c r="K83">
         <v>3817861.222171624</v>
       </c>
-      <c r="K83">
+      <c r="L83">
         <v>0.09548114246843542</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:12">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -3643,10 +3895,13 @@
       <c r="K84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:11">
+      <c r="L84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B85">
         <v>16.74</v>
@@ -3655,33 +3910,36 @@
         <v>2</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>16.74</v>
       </c>
       <c r="E85">
-        <v>16.74</v>
+        <v>0</v>
       </c>
       <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
         <v>0.04597592553328228</v>
       </c>
-      <c r="G85">
+      <c r="H85">
         <v>0.05832604257801108</v>
       </c>
-      <c r="H85">
+      <c r="I85">
         <v>1225580.246940706</v>
       </c>
-      <c r="I85">
+      <c r="J85">
         <v>777398.6585010207</v>
       </c>
-      <c r="J85">
+      <c r="K85">
         <v>2002978.905441727</v>
       </c>
-      <c r="K85">
+      <c r="L85">
         <v>0.05009263121485855</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B86">
         <v>6.23</v>
@@ -3690,33 +3948,36 @@
         <v>1</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>6.23</v>
       </c>
       <c r="E86">
-        <v>6.23</v>
+        <v>0</v>
       </c>
       <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
         <v>0.0171105146996624</v>
       </c>
-      <c r="G86">
+      <c r="H86">
         <v>0.02916302128900554</v>
       </c>
-      <c r="H86">
+      <c r="I86">
         <v>456114.9903489007</v>
       </c>
-      <c r="I86">
+      <c r="J86">
         <v>388699.3292505104</v>
       </c>
-      <c r="J86">
+      <c r="K86">
         <v>844814.319599411</v>
       </c>
-      <c r="K86">
+      <c r="L86">
         <v>0.02112801689611012</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:12">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B87">
         <v>17.11</v>
@@ -3725,33 +3986,36 @@
         <v>2</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>17.11</v>
       </c>
       <c r="E87">
-        <v>17.11</v>
+        <v>0</v>
       </c>
       <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
         <v>0.04699211982523655</v>
       </c>
-      <c r="G87">
+      <c r="H87">
         <v>0.05832604257801108</v>
       </c>
-      <c r="H87">
+      <c r="I87">
         <v>1252668.938181331</v>
       </c>
-      <c r="I87">
+      <c r="J87">
         <v>777398.6585010207</v>
       </c>
-      <c r="J87">
+      <c r="K87">
         <v>2030067.596682352</v>
       </c>
-      <c r="K87">
+      <c r="L87">
         <v>0.05077009407616139</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:12">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B88">
         <v>20.44</v>
@@ -3760,33 +4024,36 @@
         <v>2</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>20.44</v>
       </c>
       <c r="E88">
-        <v>20.44</v>
+        <v>0</v>
       </c>
       <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
         <v>0.05613786845282497</v>
       </c>
-      <c r="G88">
+      <c r="H88">
         <v>0.05832604257801108</v>
       </c>
-      <c r="H88">
+      <c r="I88">
         <v>1496467.159346955</v>
       </c>
-      <c r="I88">
+      <c r="J88">
         <v>777398.6585010207</v>
       </c>
-      <c r="J88">
+      <c r="K88">
         <v>2273865.817847976</v>
       </c>
-      <c r="K88">
+      <c r="L88">
         <v>0.05686725982788701</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:12">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -3818,10 +4085,13 @@
       <c r="K89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:11">
+      <c r="L89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -3853,10 +4123,13 @@
       <c r="K90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:11">
+      <c r="L90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -3888,10 +4161,13 @@
       <c r="K91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:11">
+      <c r="L91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -3923,10 +4199,13 @@
       <c r="K92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:11">
+      <c r="L92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -3958,10 +4237,13 @@
       <c r="K93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:11">
+      <c r="L93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -3993,10 +4275,13 @@
       <c r="K94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:11">
+      <c r="L94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -4028,10 +4313,13 @@
       <c r="K95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:11">
+      <c r="L95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -4063,10 +4351,13 @@
       <c r="K96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:11">
+      <c r="L96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -4098,10 +4389,13 @@
       <c r="K97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:11">
+      <c r="L97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -4133,10 +4427,13 @@
       <c r="K98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:11">
+      <c r="L98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
       <c r="A99" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -4166,6 +4463,9 @@
         <v>0</v>
       </c>
       <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
         <v>0</v>
       </c>
     </row>

</xml_diff>